<commit_message>
S00031 - Fix name placement issue in trimmed export
</commit_message>
<xml_diff>
--- a/tl/S00028.MES.BIN.xlsx
+++ b/tl/S00028.MES.BIN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FE9DFF-A86A-42E2-8402-56403AFAA3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC9643-41A7-44B1-995C-A9720AFF422C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="11310" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="252">
   <si>
     <t>Status</t>
   </si>
@@ -215,6 +215,12 @@
     <t>49</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Haruka</t>
+  </si>
+  <si>
     <t>Good morning. Long time no see, Yuki.</t>
   </si>
   <si>
@@ -227,12 +233,6 @@
     <t>53</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Haruka</t>
-  </si>
-  <si>
     <t>The person laughing tiredly at Yuki is &lt;c4Haruka Kawashima&gt;.</t>
   </si>
   <si>
@@ -422,6 +422,9 @@
     <t>113</t>
   </si>
   <si>
+    <t>Male Voice</t>
+  </si>
+  <si>
     <t>"Oh, good morning. Ah, Yuki is here too."</t>
   </si>
   <si>
@@ -446,6 +449,9 @@
     <t>121</t>
   </si>
   <si>
+    <t>Akira</t>
+  </si>
+  <si>
     <t>"...Submitting reports again today. Ah, sit down."</t>
   </si>
   <si>
@@ -458,9 +464,6 @@
     <t>125</t>
   </si>
   <si>
-    <t>Male Voice</t>
-  </si>
-  <si>
     <t>Yuki and I sit on the chairs that Akira recommended.</t>
   </si>
   <si>
@@ -491,9 +494,6 @@
     <t>135</t>
   </si>
   <si>
-    <t>Akira</t>
-  </si>
-  <si>
     <t>In terms of being gender-neutral, he is quite similar to Haruka.</t>
   </si>
   <si>
@@ -542,6 +542,12 @@
     <t>151</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Misaki</t>
+  </si>
+  <si>
     <t>"Ah, so it was the Fujii-kun group after all. I noticed someone who looked like them while walking outside, so I came in."</t>
   </si>
   <si>
@@ -593,12 +599,6 @@
     <t>167</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Misaki</t>
-  </si>
-  <si>
     <t>Listening to everyone's requests, Akira goes to the vending machine corner.</t>
   </si>
   <si>
@@ -771,48 +771,6 @@
   </si>
   <si>
     <t>In the end, we ended up taking a break from Akira's report work and chatted away in the discussion room for a while.</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>229</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>233</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>241</t>
-  </si>
-  <si>
-    <t>243</t>
-  </si>
-  <si>
-    <t>245</t>
-  </si>
-  <si>
-    <t>247</t>
-  </si>
-  <si>
-    <t>249</t>
-  </si>
-  <si>
-    <t>251</t>
   </si>
 </sst>
 </file>
@@ -1232,11 +1190,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1446,10 +1402,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
@@ -1478,10 +1434,10 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
@@ -1510,10 +1466,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>9</v>
@@ -1542,10 +1498,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -1574,10 +1530,10 @@
         <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
@@ -1702,10 +1658,10 @@
         <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>9</v>
@@ -1734,10 +1690,10 @@
         <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -1766,10 +1722,10 @@
         <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>9</v>
@@ -1798,10 +1754,10 @@
         <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
@@ -1830,10 +1786,10 @@
         <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>9</v>
@@ -1894,10 +1850,10 @@
         <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>9</v>
@@ -1958,10 +1914,10 @@
         <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>9</v>
@@ -2022,10 +1978,10 @@
         <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>9</v>
@@ -2054,10 +2010,10 @@
         <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>9</v>
@@ -2066,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -2083,13 +2039,13 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>9</v>
@@ -2098,7 +2054,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -2115,13 +2071,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>9</v>
@@ -2150,10 +2106,10 @@
         <v>73</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>9</v>
@@ -2310,10 +2266,10 @@
         <v>84</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>9</v>
@@ -2374,10 +2330,10 @@
         <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
@@ -2406,10 +2362,10 @@
         <v>90</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
@@ -2438,10 +2394,10 @@
         <v>92</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>9</v>
@@ -2470,10 +2426,10 @@
         <v>94</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>9</v>
@@ -2502,10 +2458,10 @@
         <v>96</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>9</v>
@@ -2566,10 +2522,10 @@
         <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>9</v>
@@ -2630,10 +2586,10 @@
         <v>105</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>9</v>
@@ -2662,10 +2618,10 @@
         <v>107</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>9</v>
@@ -2694,10 +2650,10 @@
         <v>109</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>9</v>
@@ -2726,10 +2682,10 @@
         <v>112</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>9</v>
@@ -2790,10 +2746,10 @@
         <v>116</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>9</v>
@@ -2854,10 +2810,10 @@
         <v>120</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>9</v>
@@ -2886,10 +2842,10 @@
         <v>122</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>9</v>
@@ -2950,10 +2906,10 @@
         <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>9</v>
@@ -3078,10 +3034,10 @@
         <v>134</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>9</v>
@@ -3090,7 +3046,7 @@
         <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>9</v>
@@ -3107,7 +3063,7 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
@@ -3122,7 +3078,7 @@
         <v>9</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -3139,13 +3095,13 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>9</v>
@@ -3154,7 +3110,7 @@
         <v>9</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>9</v>
@@ -3171,7 +3127,7 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
@@ -3186,7 +3142,7 @@
         <v>9</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3203,13 +3159,13 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
@@ -3218,7 +3174,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3235,13 +3191,13 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>9</v>
@@ -3250,7 +3206,7 @@
         <v>9</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3267,13 +3223,13 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>9</v>
@@ -3282,7 +3238,7 @@
         <v>9</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3299,13 +3255,13 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
@@ -3314,7 +3270,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3331,13 +3287,13 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>9</v>
@@ -3346,7 +3302,7 @@
         <v>9</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3363,7 +3319,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3378,7 +3334,7 @@
         <v>9</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3395,7 +3351,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>9</v>
@@ -3410,7 +3366,7 @@
         <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>9</v>
@@ -3427,13 +3383,13 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>9</v>
@@ -3462,10 +3418,10 @@
         <v>160</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>9</v>
@@ -3497,7 +3453,7 @@
         <v>9</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
@@ -3526,10 +3482,10 @@
         <v>164</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>9</v>
@@ -3561,7 +3517,7 @@
         <v>9</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>9</v>
@@ -3590,10 +3546,10 @@
         <v>168</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>9</v>
@@ -3686,10 +3642,10 @@
         <v>174</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>9</v>
@@ -3698,10 +3654,10 @@
         <v>9</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>9</v>
@@ -3715,13 +3671,13 @@
         <v>9</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>9</v>
@@ -3730,7 +3686,7 @@
         <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>9</v>
@@ -3747,13 +3703,13 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>9</v>
@@ -3762,7 +3718,7 @@
         <v>9</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>9</v>
@@ -3779,13 +3735,13 @@
         <v>9</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>9</v>
@@ -3794,7 +3750,7 @@
         <v>9</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>9</v>
@@ -3811,7 +3767,7 @@
         <v>9</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>9</v>
@@ -3826,7 +3782,7 @@
         <v>9</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -3843,13 +3799,13 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>9</v>
@@ -3858,7 +3814,7 @@
         <v>9</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -3875,7 +3831,7 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>9</v>
@@ -3890,7 +3846,7 @@
         <v>9</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -3907,13 +3863,13 @@
         <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>9</v>
@@ -3922,7 +3878,7 @@
         <v>9</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -3939,13 +3895,13 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>9</v>
@@ -3974,10 +3930,10 @@
         <v>195</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
@@ -4006,10 +3962,10 @@
         <v>198</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>9</v>
@@ -4038,10 +3994,10 @@
         <v>200</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>9</v>
@@ -4166,10 +4122,10 @@
         <v>208</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>9</v>
@@ -4198,10 +4154,10 @@
         <v>210</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>9</v>
@@ -4233,7 +4189,7 @@
         <v>9</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>9</v>
@@ -4422,10 +4378,10 @@
         <v>224</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>9</v>
@@ -4454,10 +4410,10 @@
         <v>226</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>9</v>
@@ -4486,10 +4442,10 @@
         <v>228</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>22</v>
+        <v>175</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>23</v>
+        <v>176</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>9</v>
@@ -4518,10 +4474,10 @@
         <v>230</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>9</v>
@@ -4550,10 +4506,10 @@
         <v>232</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>9</v>
@@ -4617,7 +4573,7 @@
         <v>9</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>9</v>
@@ -4710,10 +4666,10 @@
         <v>242</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>9</v>
@@ -4745,7 +4701,7 @@
         <v>9</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>9</v>
@@ -4838,10 +4794,10 @@
         <v>250</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>9</v>
@@ -4859,454 +4815,6 @@
         <v>9</v>
       </c>
       <c r="J113" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J114" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G115" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H115" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I115" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J115" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H117" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I117" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J117" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J118" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G119" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I119" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J119" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H121" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I121" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J121" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D123" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E123" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G123" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I123" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J123" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J124" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G125" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H125" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I125" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J125" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H126" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J126" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D127" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F127" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G127" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H127" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I127" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J127" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Support for choices (new font patch change) - S00035, 36, 37, 50, 51, 52, 55
</commit_message>
<xml_diff>
--- a/tl/S00028.MES.BIN.xlsx
+++ b/tl/S00028.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC9643-41A7-44B1-995C-A9720AFF422C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DC8BEF-5B3E-42F7-BA7E-3D25CA4EA08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="11310" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="10155" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00028.MES.BIN" sheetId="1" r:id="rId1"/>

</xml_diff>